<commit_message>
Actualización de mi logt
</commit_message>
<xml_diff>
--- a/tspi/ciclo-4/plan4-20106065.xlsx
+++ b/tspi/ciclo-4/plan4-20106065.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="-45" windowWidth="9540" windowHeight="7365" tabRatio="400"/>
+    <workbookView xWindow="9660" yWindow="-45" windowWidth="9540" windowHeight="7365" tabRatio="486"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Id</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>Cada miembro del equipo completó la forma PEER. Se creó el reporte del ciclo correspondiente. Se completaron las formas SUMP y SUMQ para el sistema y todos sus componentes.</t>
+  </si>
+  <si>
+    <t>Elabore el plan del ciclo #4.</t>
+  </si>
+  <si>
+    <t>Realize el lanzamiento del ciclo #4.</t>
   </si>
 </sst>
 </file>
@@ -665,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALY9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5990,7 +5996,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6013,17 +6019,28 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
+      <c r="A2" s="4">
+        <v>64</v>
+      </c>
       <c r="B2" s="4">
         <f>SUMIF(logt!G:G,task!A2,logt!F:F)/60</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="4"/>
+        <v>1.4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="4">
+        <v>62</v>
+      </c>
+      <c r="B3" s="4">
+        <f>SUMIF(logt!G:G,task!A3,logt!F:F)/60</f>
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="C3" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
@@ -6108,7 +6125,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6150,14 +6167,58 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="19">
+        <v>41962</v>
+      </c>
+      <c r="B2" s="17">
+        <v>9</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0.4368055555555555</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0</v>
+      </c>
       <c r="F2" s="12">
-        <f t="shared" ref="F2" si="0">((HOUR(D2)-HOUR(C2))*60)+(MINUTE(D2)-MINUTE(C2))-E2</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="27"/>
+        <f t="shared" ref="F2:F3" si="0">((HOUR(D2)-HOUR(C2))*60)+(MINUTE(D2)-MINUTE(C2))-E2</f>
+        <v>84</v>
+      </c>
+      <c r="G2" s="17">
+        <v>64</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H3" s="28"/>
+      <c r="A3" s="19">
+        <v>41962</v>
+      </c>
+      <c r="B3" s="17">
+        <v>9</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0.4375</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.45763888888888887</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="G3" s="17">
+        <v>62</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20"/>

</xml_diff>

<commit_message>
Actualizacion de mi logt
</commit_message>
<xml_diff>
--- a/tspi/ciclo-4/plan4-20106065.xlsx
+++ b/tspi/ciclo-4/plan4-20106065.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>Id</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Reasignando las tareas del plan.</t>
+  </si>
+  <si>
+    <t>Defini los cambios que deben hacerse para la implementacion de la funcionalidad #4.</t>
   </si>
 </sst>
 </file>
@@ -465,8 +468,8 @@
   </sheetPr>
   <dimension ref="1:8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4967,10 +4970,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:19"/>
+  <dimension ref="1:20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10562,6 +10565,33 @@
         <v>41</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="28" t="n">
+        <v>41939</v>
+      </c>
+      <c r="B20" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" s="29" t="n">
+        <v>0.4125</v>
+      </c>
+      <c r="D20" s="29" t="n">
+        <v>0.484722222222222</v>
+      </c>
+      <c r="E20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="24" t="n">
+        <f aca="false">((HOUR(D20)-HOUR(C20))*60)+(MINUTE(D20)-MINUTE(C20))-E20</f>
+        <v>104</v>
+      </c>
+      <c r="G20" s="7" t="n">
+        <v>74</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Actualización de las gráficas generales del proyecto
</commit_message>
<xml_diff>
--- a/tspi/ciclo-4/plan4-20106065.xlsx
+++ b/tspi/ciclo-4/plan4-20106065.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="486" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="922" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Id</t>
   </si>
@@ -469,7 +469,7 @@
   <dimension ref="1:8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -798,10 +798,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:5"/>
+  <dimension ref="1:6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3921,7 +3921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="n">
         <v>61</v>
       </c>
@@ -4954,6 +4954,18 @@
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>70</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <f aca="false">SUMIF(logt!G:G,task!A6,logt!F:F)/60</f>
+        <v>13.6166666666667</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4970,10 +4982,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:20"/>
+  <dimension ref="1:21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10486,7 +10498,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="27" t="n">
-        <v>41937</v>
+        <v>41968</v>
       </c>
       <c r="B17" s="22" t="n">
         <v>10</v>
@@ -10513,7 +10525,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="n">
-        <v>41937</v>
+        <v>41968</v>
       </c>
       <c r="B18" s="7" t="n">
         <v>10</v>
@@ -10540,7 +10552,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="28" t="n">
-        <v>41937</v>
+        <v>41968</v>
       </c>
       <c r="B19" s="7" t="n">
         <v>10</v>
@@ -10567,7 +10579,7 @@
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="28" t="n">
-        <v>41939</v>
+        <v>41970</v>
       </c>
       <c r="B20" s="7" t="n">
         <v>10</v>
@@ -10590,6 +10602,30 @@
       </c>
       <c r="H20" s="2" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="28" t="n">
+        <v>41970</v>
+      </c>
+      <c r="B21" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="C21" s="29" t="n">
+        <v>0.638194444444444</v>
+      </c>
+      <c r="D21" s="29" t="n">
+        <v>0.681944444444444</v>
+      </c>
+      <c r="E21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="24" t="n">
+        <f aca="false">((HOUR(D21)-HOUR(C21))*60)+(MINUTE(D21)-MINUTE(C21))-E21</f>
+        <v>63</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion del sistema de archivos
</commit_message>
<xml_diff>
--- a/tspi/ciclo-4/plan4-20106065.xlsx
+++ b/tspi/ciclo-4/plan4-20106065.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>Id</t>
   </si>
@@ -5009,10 +5009,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:30"/>
+  <dimension ref="1:31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10861,6 +10861,7 @@
         <f aca="false">((HOUR(D29)-HOUR(C29))*60)+(MINUTE(D29)-MINUTE(C29))-E29</f>
         <v>55</v>
       </c>
+      <c r="G29" s="0"/>
       <c r="H29" s="2" t="s">
         <v>47</v>
       </c>
@@ -10889,6 +10890,33 @@
         <v>76</v>
       </c>
       <c r="H30" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="28" t="n">
+        <v>41976</v>
+      </c>
+      <c r="B31" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="C31" s="29" t="n">
+        <v>0.631944444444444</v>
+      </c>
+      <c r="D31" s="29" t="n">
+        <v>0.701388888888889</v>
+      </c>
+      <c r="E31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="24" t="n">
+        <f aca="false">((HOUR(D31)-HOUR(C31))*60)+(MINUTE(D31)-MINUTE(C31))-E31</f>
+        <v>100</v>
+      </c>
+      <c r="G31" s="7" t="n">
+        <v>76</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>